<commit_message>
saving the experiments externaly to save space and applyed a syncing funtion to load the experiments results from DFKI cluster
</commit_message>
<xml_diff>
--- a/run_metrics.xlsx
+++ b/run_metrics.xlsx
@@ -29,7 +29,7 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
@@ -40,6 +40,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="00FFFF00"/>
         <bgColor rgb="00FFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0090EE90"/>
+        <bgColor rgb="0090EE90"/>
       </patternFill>
     </fill>
   </fills>
@@ -61,12 +67,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -432,7 +439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,293 +467,293 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>AttentionUNet_LFCC_32_len5S</t>
+          <t>R2AttU_Net_lfcc-delta_32_len5S</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>67.39130434782609</v>
+        <v>69.56521739130434</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5579307675361633</v>
+        <v>0.557578980922699</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>AttentionUNet_lfcc-delta-delta_32_len5S</t>
+          <t>U_Net_delta_32_len30S</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>73.91304347826087</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.5381553471088409</v>
+        <v>0</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>U_Net_lfcc-delta-delta_32_len5S</t>
+          <t>U_Net_delta_32_len30S</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>76.08695652173913</v>
+        <v>93.47826086956522</v>
       </c>
       <c r="C4" t="n">
-        <v>0.5723033547401428</v>
+        <v>0.8856147925059</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>R2AttU_Net_MFCC_32_len5S</t>
+          <t>U_Net_delta_32_len30S</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>69.56521739130434</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0.5817689299583435</v>
+        <v>0</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>R2AttU_Net_delta-delta_32_len5S</t>
+          <t>U_Net_LFCC_80_len5S</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>73.91304347826087</v>
+        <v>91.30434782608695</v>
       </c>
       <c r="C6" t="n">
-        <v>0.6064977645874023</v>
+        <v>0.8510100543498993</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>U_Net_delta_80_len5S</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>69.56521739130434</v>
+          <t>U_Net_LFCC_32_len5S</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>95.65217391304348</v>
       </c>
       <c r="C7" t="n">
-        <v>0.6144457757472992</v>
+        <v>0.8168511788050333</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>U_Net_lfcc-delta-delta_32_len30S</t>
+          <t>AttentionUNet_lfcc-delta-delta_32_len5S</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+        <v>76.08695652173913</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.5528329908847809</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>U_Net_LFCC_32_len5S</t>
+          <t>AttentionUNet_MFCC_32_len5S</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>73.91304347826087</v>
+        <v>67.39130434782609</v>
       </c>
       <c r="C9" t="n">
-        <v>0.5816247860590616</v>
+        <v>0.5642368793487549</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>U_Net_delta_32_len30S</t>
+          <t>U_Net_MFCC_32_len5S</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>67.39130434782609</v>
+        <v>86.95652173913044</v>
       </c>
       <c r="C10" t="n">
-        <v>0.5975880722204844</v>
+        <v>0.9281513889630636</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>U_Net_delta_32_len30S</t>
+          <t>AttentionUNet_delta_32_len5S</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+        <v>82.60869565217391</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.5391703248023987</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>U_Net_delta_32_len5S</t>
+          <t>R2U_Net_LFCC_32_len5S</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>63.04347826086956</v>
+        <v>73.91304347826087</v>
       </c>
       <c r="C12" t="n">
-        <v>0.6578056216239929</v>
+        <v>0.6428556889295578</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>U_Net_MFCC_80_len5S</t>
+          <t>U_Net_lfcc-delta-delta_32_len5S</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>76.08695652173913</v>
+        <v>78.26086956521739</v>
       </c>
       <c r="C13" t="n">
-        <v>0.6022742092609406</v>
+        <v>0.9822227358818054</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>U_Net_lfcc-delta_32_len30S</t>
+          <t>R2U_Net_delta_32_len5S</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>71.73913043478261</v>
+        <v>73.91304347826087</v>
       </c>
       <c r="C14" t="n">
-        <v>0.6148889064788818</v>
+        <v>0.5048011690378189</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>U_Net_lfcc-delta_32_len30S</t>
+          <t>R2AttU_Net_MFCC_32_len5S</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0</v>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+        <v>76.08695652173913</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.5616060495376587</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>R2AttU_Net_delta_32_len5S</t>
+          <t>U_Net_delta_32_len5S</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>78.26086956521739</v>
+        <v>71.73913043478261</v>
       </c>
       <c r="C16" t="n">
-        <v>0.5247934460639954</v>
+        <v>1.076469659805298</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>AttentionUNet_lfcc-delta_32_len5S</t>
+          <t>R2AttU_Net_delta_32_len5S</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>73.91304347826087</v>
+        <v>69.56521739130434</v>
       </c>
       <c r="C17" t="n">
-        <v>0.5427097231149673</v>
+        <v>0.5860709249973297</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>U_Net_delta-delta_32_len5S</t>
+          <t>U_Net_delta_80_len5S</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>58.69565217391305</v>
+        <v>63.04347826086956</v>
       </c>
       <c r="C18" t="n">
-        <v>0.6423204143842062</v>
+        <v>1.033747345209122</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>R2U_Net_delta_32_len5S</t>
+          <t>U_Net_MFCC_32_len30S</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>78.26086956521739</v>
+        <v>89.1304347826087</v>
       </c>
       <c r="C19" t="n">
-        <v>0.5741766691207886</v>
+        <v>0.8510035673777262</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>R2AttU_Net_lfcc-delta-delta_32_len5S</t>
+          <t>U_Net_MFCC_32_len30S</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>71.73913043478261</v>
+        <v>86.95652173913044</v>
       </c>
       <c r="C20" t="n">
-        <v>0.6232963800430298</v>
+        <v>0.8733596205711365</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>U_Net_lfcc-delta_32_len5S</t>
+          <t>U_Net_MFCC_32_len30S</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>78.26086956521739</v>
-      </c>
-      <c r="C21" t="n">
-        <v>0.5364510814348856</v>
+        <v>0</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>R2U_Net_delta-delta_32_len5S</t>
+          <t>AttentionUNet_LFCC_32_len5S</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>69.56521739130434</v>
-      </c>
-      <c r="C22" t="n">
-        <v>0.6311409175395966</v>
+        <v>82.60869565217391</v>
+      </c>
+      <c r="C22" s="3" t="n">
+        <v>0.4653773456811905</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>R2AttU_Net_lfcc-delta_32_len5S</t>
+          <t>R2AttU_Net_lfcc-delta-delta_32_len5S</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>58.69565217391305</v>
+        <v>54.34782608695652</v>
       </c>
       <c r="C23" t="n">
-        <v>0.6667028069496155</v>
+        <v>0.6629349291324615</v>
       </c>
     </row>
     <row r="24">
@@ -756,57 +763,57 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>71.73913043478261</v>
+        <v>89.1304347826087</v>
       </c>
       <c r="C24" t="n">
-        <v>0.5703217685222626</v>
+        <v>0.9213963150978088</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>U_Net_MFCC_32_len30S</t>
+          <t>R2U_Net_MFCC_32_len5S</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>80.43478260869566</v>
+        <v>50</v>
       </c>
       <c r="C25" t="n">
-        <v>0.4891441067059835</v>
+        <v>0.6707836836576462</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>U_Net_MFCC_32_len30S</t>
+          <t>U_Net_delta-delta_32_len30S</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0</v>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+        <v>78.26086956521739</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.9564621647198995</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>U_Net_LFCC_32_len30S</t>
-        </is>
-      </c>
-      <c r="B27" s="2" t="n">
-        <v>84.78260869565217</v>
-      </c>
-      <c r="C27" t="n">
-        <v>0.46284352739652</v>
+          <t>U_Net_delta-delta_32_len30S</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>0</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>U_Net_LFCC_32_len30S</t>
+          <t>U_Net_lfcc-delta-delta_32_len30S</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -821,81 +828,226 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>AttentionUNet_delta_32_len5S</t>
+          <t>U_Net_lfcc-delta-delta_32_len30S</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>69.56521739130434</v>
+        <v>63.04347826086956</v>
       </c>
       <c r="C29" t="n">
-        <v>0.5166951715946198</v>
+        <v>1.059326450030009</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>U_Net_delta-delta_32_len30S</t>
+          <t>U_Net_delta-delta_32_len5S</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0</v>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+        <v>63.04347826086956</v>
+      </c>
+      <c r="C30" t="n">
+        <v>1.100150108337402</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>U_Net_delta-delta_32_len30S</t>
+          <t>U_Net_lfcc-delta_32_len30S</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>73.91304347826087</v>
-      </c>
-      <c r="C31" t="n">
-        <v>0.5577747623125712</v>
+        <v>0</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>AttentionUNet_MFCC_32_len5S</t>
+          <t>U_Net_lfcc-delta_32_len30S</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>73.91304347826087</v>
+        <v>84.78260869565217</v>
       </c>
       <c r="C32" t="n">
-        <v>0.5551608800888062</v>
+        <v>0.9093547463417053</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>AttentionUNet_delta-delta_32_len5S</t>
+          <t>U_Net_LFCC_32_len30S</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>65.21739130434783</v>
+        <v>86.95652173913044</v>
       </c>
       <c r="C33" t="n">
-        <v>0.623989462852478</v>
+        <v>0.8723922967910767</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
+          <t>U_Net_LFCC_32_len30S</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>0</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>R2U_Net_lfcc-delta_32_len5S</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>78.26086956521739</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0.5619004666805267</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>R2AttU_Net_delta-delta_32_len5S</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>58.69565217391305</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0.665488988161087</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>R2U_Net_lfcc-delta-delta_32_len5S</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>67.39130434782609</v>
+      </c>
+      <c r="C37" t="n">
+        <v>0.5734604299068451</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>R2AttU_Net_LFCC_32_len5S</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>73.91304347826087</v>
+      </c>
+      <c r="C38" t="n">
+        <v>0.533536896109581</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>AttentionUNet_lfcc-delta_32_len5S</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>78.26086956521739</v>
+      </c>
+      <c r="C39" t="n">
+        <v>0.5578003972768784</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>U_Net_lfcc-delta_80_len5S</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>93.47826086956522</v>
+      </c>
+      <c r="C40" t="n">
+        <v>0.8924888968467712</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>R2U_Net_delta-delta_32_len5S</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>73.91304347826087</v>
+      </c>
+      <c r="C41" t="n">
+        <v>0.621788889169693</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
           <t>U_Net_delta-delta_80_len5S</t>
         </is>
       </c>
-      <c r="B34" t="n">
-        <v>54.34782608695652</v>
-      </c>
-      <c r="C34" t="n">
-        <v>0.6456651091575623</v>
+      <c r="B42" t="n">
+        <v>50</v>
+      </c>
+      <c r="C42" t="n">
+        <v>1.081704556941986</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>AttentionUNet_delta-delta_32_len5S</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>60.8695652173913</v>
+      </c>
+      <c r="C43" t="n">
+        <v>0.5899332761764526</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>U_Net_MFCC_80_len5S</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>78.26086956521739</v>
+      </c>
+      <c r="C44" t="n">
+        <v>0.9191123247146606</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>U_Net_lfcc-delta_32_len5S</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>67.39130434782609</v>
+      </c>
+      <c r="C45" t="n">
+        <v>1.047885318597158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>